<commit_message>
updated some canges i index.php and store detais page
</commit_message>
<xml_diff>
--- a/documentation/credentials.xlsx
+++ b/documentation/credentials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>WheelPact Hosting Details</t>
   </si>
@@ -130,6 +130,27 @@
   </si>
   <si>
     <t>154.41.233.236</t>
+  </si>
+  <si>
+    <t>SMTP Details</t>
+  </si>
+  <si>
+    <t>Host</t>
+  </si>
+  <si>
+    <t>smtp.hostinger.com</t>
+  </si>
+  <si>
+    <t>info@parastoneglobal-ksa.com</t>
+  </si>
+  <si>
+    <t>info@paraSKSA321#</t>
+  </si>
+  <si>
+    <t>Email Details</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
 </sst>
 </file>
@@ -483,27 +504,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="88.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="88.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>19</v>
@@ -512,7 +533,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>21</v>
@@ -521,14 +542,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>23</v>
@@ -537,7 +558,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>24</v>
@@ -546,7 +567,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>27</v>
@@ -555,7 +576,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>28</v>
@@ -564,7 +585,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>30</v>
@@ -573,7 +594,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>31</v>
@@ -582,14 +603,14 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>16</v>
@@ -598,7 +619,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -609,7 +630,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>2</v>
@@ -618,7 +639,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>3</v>
@@ -627,7 +648,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
         <v>4</v>
@@ -636,7 +657,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>5</v>
@@ -645,14 +666,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>10</v>
@@ -661,7 +682,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>9</v>
@@ -670,7 +691,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>3</v>
@@ -679,7 +700,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>4</v>
@@ -688,14 +709,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
         <v>16</v>
@@ -704,7 +725,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
         <v>3</v>
@@ -713,13 +734,77 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>